<commit_message>
added new samples and conflicts
</commit_message>
<xml_diff>
--- a/conflicts.xlsx
+++ b/conflicts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wbjc/Documents/Jakki_Dokumente/RaspiSamplePlayer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wbjc/Documents/Jakki_Dokumente/RSP/RSP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3DFEC9-3A8D-864B-B78F-3E794BDA31ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69D89E4-DB6A-0648-B4CB-1EFC8AF8B1D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14700" xr2:uid="{9C425E25-B675-FA47-820B-67817447EAF8}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="14700" xr2:uid="{9C425E25-B675-FA47-820B-67817447EAF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -87,9 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -404,15 +406,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E890110B-7CE3-5948-9F7A-FBF2710AFED1}">
-  <dimension ref="A1:B272"/>
+  <dimension ref="A1:B308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B272"/>
+      <selection activeCell="F280" sqref="F280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2591,7 +2594,296 @@
         <v>52</v>
       </c>
     </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="3">
+        <v>78</v>
+      </c>
+      <c r="B273" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="3">
+        <v>79</v>
+      </c>
+      <c r="B274" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>82</v>
+      </c>
+      <c r="B275" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>83</v>
+      </c>
+      <c r="B276" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
+        <v>84</v>
+      </c>
+      <c r="B277" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="3">
+        <v>85</v>
+      </c>
+      <c r="B278" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="3">
+        <v>85</v>
+      </c>
+      <c r="B279" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="3">
+        <v>85</v>
+      </c>
+      <c r="B280" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="3">
+        <v>85</v>
+      </c>
+      <c r="B281" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="3">
+        <v>85</v>
+      </c>
+      <c r="B282" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="3">
+        <v>85</v>
+      </c>
+      <c r="B283" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="3">
+        <v>85</v>
+      </c>
+      <c r="B284" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="3">
+        <v>85</v>
+      </c>
+      <c r="B285" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="3">
+        <v>85</v>
+      </c>
+      <c r="B286" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="3">
+        <v>85</v>
+      </c>
+      <c r="B287" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="3">
+        <v>85</v>
+      </c>
+      <c r="B288" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="3">
+        <v>85</v>
+      </c>
+      <c r="B289" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="3">
+        <v>85</v>
+      </c>
+      <c r="B290" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A291" s="3">
+        <v>85</v>
+      </c>
+      <c r="B291" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A292" s="3">
+        <v>85</v>
+      </c>
+      <c r="B292" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" s="3">
+        <v>85</v>
+      </c>
+      <c r="B293" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" s="3">
+        <v>85</v>
+      </c>
+      <c r="B294" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A295" s="3">
+        <v>85</v>
+      </c>
+      <c r="B295" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A296" s="3">
+        <v>85</v>
+      </c>
+      <c r="B296" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A297" s="3">
+        <v>85</v>
+      </c>
+      <c r="B297" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A298" s="3">
+        <v>85</v>
+      </c>
+      <c r="B298" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A299" s="3">
+        <v>85</v>
+      </c>
+      <c r="B299" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" s="3">
+        <v>85</v>
+      </c>
+      <c r="B300" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A301" s="3">
+        <v>85</v>
+      </c>
+      <c r="B301" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A302" s="3">
+        <v>85</v>
+      </c>
+      <c r="B302" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A303" s="3">
+        <v>85</v>
+      </c>
+      <c r="B303" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A304" s="3">
+        <v>85</v>
+      </c>
+      <c r="B304" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" s="3">
+        <v>85</v>
+      </c>
+      <c r="B305" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" s="3">
+        <v>85</v>
+      </c>
+      <c r="B306" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" s="3">
+        <v>85</v>
+      </c>
+      <c r="B307" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="3">
+        <v>85</v>
+      </c>
+      <c r="B308" s="2">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
neue samples in die listen eingefuegt
</commit_message>
<xml_diff>
--- a/conflicts.xlsx
+++ b/conflicts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wbjc/Documents/Jakki_Dokumente/RSP/RSP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69D89E4-DB6A-0648-B4CB-1EFC8AF8B1D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC60047-104A-5E49-87B3-D7805CC9BE84}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="14700" xr2:uid="{9C425E25-B675-FA47-820B-67817447EAF8}"/>
+    <workbookView xWindow="580" yWindow="1280" windowWidth="25020" windowHeight="14700" xr2:uid="{9C425E25-B675-FA47-820B-67817447EAF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E890110B-7CE3-5948-9F7A-FBF2710AFED1}">
-  <dimension ref="A1:B308"/>
+  <dimension ref="A1:B329"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F280" sqref="F280"/>
+      <selection activeCell="B330" sqref="B330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2882,6 +2882,174 @@
         <v>64</v>
       </c>
     </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" s="3">
+        <v>86</v>
+      </c>
+      <c r="B309" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="3">
+        <v>86</v>
+      </c>
+      <c r="B310" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="3">
+        <v>86</v>
+      </c>
+      <c r="B311" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" s="3">
+        <v>87</v>
+      </c>
+      <c r="B312" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A313" s="3">
+        <v>87</v>
+      </c>
+      <c r="B313" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" s="3">
+        <v>87</v>
+      </c>
+      <c r="B314" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A315" s="3">
+        <v>87</v>
+      </c>
+      <c r="B315" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A316" s="3">
+        <v>87</v>
+      </c>
+      <c r="B316" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A317" s="3">
+        <v>87</v>
+      </c>
+      <c r="B317" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A318" s="3">
+        <v>87</v>
+      </c>
+      <c r="B318" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" s="3">
+        <v>87</v>
+      </c>
+      <c r="B319" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A320" s="3">
+        <v>87</v>
+      </c>
+      <c r="B320" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="3">
+        <v>88</v>
+      </c>
+      <c r="B321" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="3">
+        <v>88</v>
+      </c>
+      <c r="B322" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A323" s="3">
+        <v>88</v>
+      </c>
+      <c r="B323" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" s="3">
+        <v>88</v>
+      </c>
+      <c r="B324" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" s="3">
+        <v>88</v>
+      </c>
+      <c r="B325" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A326" s="3">
+        <v>88</v>
+      </c>
+      <c r="B326" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" s="3">
+        <v>88</v>
+      </c>
+      <c r="B327" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" s="3">
+        <v>88</v>
+      </c>
+      <c r="B328" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A329" s="3">
+        <v>88</v>
+      </c>
+      <c r="B329" s="3">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added more samples to excel files
</commit_message>
<xml_diff>
--- a/conflicts.xlsx
+++ b/conflicts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wbjc/Documents/Jakki_Dokumente/RSP/RSP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC60047-104A-5E49-87B3-D7805CC9BE84}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F936B3F7-0BAF-4A40-A8AE-120FFCBB7118}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1280" windowWidth="25020" windowHeight="14700" xr2:uid="{9C425E25-B675-FA47-820B-67817447EAF8}"/>
+    <workbookView xWindow="19300" yWindow="1220" windowWidth="21360" windowHeight="14700" xr2:uid="{9C425E25-B675-FA47-820B-67817447EAF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -83,15 +83,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -406,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E890110B-7CE3-5948-9F7A-FBF2710AFED1}">
-  <dimension ref="A1:B329"/>
+  <dimension ref="A1:B351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B330" sqref="B330"/>
+    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="A351" sqref="A351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3050,6 +3062,182 @@
         <v>70</v>
       </c>
     </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" s="4">
+        <v>89</v>
+      </c>
+      <c r="B330" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A331" s="4">
+        <v>89</v>
+      </c>
+      <c r="B331" s="4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" s="4">
+        <v>89</v>
+      </c>
+      <c r="B332" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" s="4">
+        <v>89</v>
+      </c>
+      <c r="B333" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A334" s="4">
+        <v>89</v>
+      </c>
+      <c r="B334" s="4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" s="4">
+        <v>89</v>
+      </c>
+      <c r="B335" s="4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" s="4">
+        <v>89</v>
+      </c>
+      <c r="B336" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A337" s="4">
+        <v>143</v>
+      </c>
+      <c r="B337" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A338" s="4">
+        <v>143</v>
+      </c>
+      <c r="B338" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A339" s="4">
+        <v>143</v>
+      </c>
+      <c r="B339" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A340" s="4">
+        <v>143</v>
+      </c>
+      <c r="B340" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A341" s="4">
+        <v>143</v>
+      </c>
+      <c r="B341" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A342" s="4">
+        <v>193</v>
+      </c>
+      <c r="B342" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A343" s="4">
+        <v>202</v>
+      </c>
+      <c r="B343" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" s="4">
+        <v>202</v>
+      </c>
+      <c r="B344" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A345" s="4">
+        <v>202</v>
+      </c>
+      <c r="B345" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A346" s="4">
+        <v>202</v>
+      </c>
+      <c r="B346" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A347" s="4">
+        <v>202</v>
+      </c>
+      <c r="B347" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A348" s="4">
+        <v>202</v>
+      </c>
+      <c r="B348" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A349" s="4">
+        <v>202</v>
+      </c>
+      <c r="B349" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A350" s="4">
+        <v>202</v>
+      </c>
+      <c r="B350" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A351" s="4">
+        <v>93</v>
+      </c>
+      <c r="B351" s="4">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>